<commit_message>
Some lines in the documents are editted Signed-off-by: mostafamoh1236 <mostafamoh1236@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ/SIQ.xlsx
+++ b/Input documents/SIQ/SIQ.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Request ID</t>
   </si>
@@ -43,13 +43,22 @@
   </si>
   <si>
     <t>Submission Date</t>
+  </si>
+  <si>
+    <t>REQ_ PO2_EBL_Electric_Blender_SRS_001.3-1.0</t>
+  </si>
+  <si>
+    <t>Mostafa Ramadan</t>
+  </si>
+  <si>
+    <t>what should be the speed for each state?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +79,21 @@
       <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -98,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -107,6 +131,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -381,7 +413,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,15 +423,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" customWidth="1"/>
     <col min="4" max="4" width="52.28515625" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
@@ -434,10 +466,22 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="47.45" customHeight="1">
-      <c r="C2" s="3"/>
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="6">
+        <v>43854</v>
+      </c>
+      <c r="F2" s="6">
+        <v>43854</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>

</xml_diff>

<commit_message>
Answer the questions in SIQ sheet Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ/SIQ.xlsx
+++ b/Input documents/SIQ/SIQ.xlsx
@@ -131,6 +131,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -297,20 +298,20 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="49.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="49.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Reviewing the CYRS and Editing the SRS
Reviewing the CYRS document and releasing it with editing the SRS with respect to the review and the feedback that was given to the other documents.
</commit_message>
<xml_diff>
--- a/Input documents/SIQ/SIQ.xlsx
+++ b/Input documents/SIQ/SIQ.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Documents\GitHub\GroupA_Electric_Blender-ITI-Intake40-\Input documents\SIQ\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,58 +24,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">Request ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asked by</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Request ID</t>
+  </si>
+  <si>
+    <t>Asked by</t>
   </si>
   <si>
     <t xml:space="preserve">Question </t>
   </si>
   <si>
-    <t xml:space="preserve">Proposed Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submission Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected Response Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REQ_ PO2_EBL_Electric_Blender_SRS_001.3-1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mostafa Ramadan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what should be the speed for each state?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/1/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speed 1 : from 0% up to 30%. 
+    <t>Proposed Answer</t>
+  </si>
+  <si>
+    <t>Submission Date</t>
+  </si>
+  <si>
+    <t>Expected Response Date</t>
+  </si>
+  <si>
+    <t>Return Date</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>REQ_ PO2_EBL_Electric_Blender_SRS_001.3-1.0</t>
+  </si>
+  <si>
+    <t>Mostafa Ramadan</t>
+  </si>
+  <si>
+    <t>what should be the speed for each state?</t>
+  </si>
+  <si>
+    <t>30/1/2020</t>
+  </si>
+  <si>
+    <t>Speed 1 : from 0% up to 30%. 
 Speed 2: above 30% up to 60%. 
 Speed 3: above  60 % up to 100%.</t>
+  </si>
+  <si>
+    <t>What is the defined voltage at which the system would be cosidered failed ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -80,22 +86,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="18"/>
       <color rgb="FF333F50"/>
       <name val="Times New Roman"/>
@@ -103,7 +94,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
@@ -111,7 +102,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -119,7 +110,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -130,7 +121,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -149,7 +139,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -157,77 +147,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -286,35 +239,309 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333F50"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="49.87"/>
+    <col min="1" max="1" width="55.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" customWidth="1"/>
+    <col min="6" max="6" width="38" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1"/>
+    <col min="8" max="8" width="70.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="46.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -340,7 +567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -351,10 +578,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="7">
         <v>43854</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="7">
         <v>43854</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -364,15 +591,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G3" s="9">
+        <v>44014</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -380,7 +611,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -388,7 +619,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -396,7 +627,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -404,7 +635,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -412,7 +643,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -420,7 +651,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -428,7 +659,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -436,7 +667,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -444,7 +675,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -452,7 +683,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -460,7 +691,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -468,7 +699,7 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -476,7 +707,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="3:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -484,7 +715,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="3:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -492,7 +723,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="3:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -500,7 +731,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="3:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -508,7 +739,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="3:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -516,7 +747,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="3:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -524,7 +755,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="3:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -532,7 +763,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="3:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -540,7 +771,7 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="47.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="3:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -549,12 +780,7 @@
       <c r="H25" s="6"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- in SIQ: Add a question regarding the PWM frequency considered a private API or not - in GDD: re-arrange the requirement IDs of the GDD APIs Signed-off-by: mostafamoh1236 <mostafamoh1236@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/SIQ/SIQ.xlsx
+++ b/Input documents/SIQ/SIQ.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,59 +19,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">Request ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asked by</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+  <si>
+    <t>Request ID</t>
+  </si>
+  <si>
+    <t>Asked by</t>
   </si>
   <si>
     <t xml:space="preserve">Question </t>
   </si>
   <si>
-    <t xml:space="preserve">Proposed Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submission Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expected Response Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Return Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Answer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REQ_ PO2_EBL_Electric_Blender_SRS_001.3-1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mostafa Ramadan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what should be the speed for each state?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/1/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speed 1 : from 0% up to 30%. 
+    <t>Proposed Answer</t>
+  </si>
+  <si>
+    <t>Submission Date</t>
+  </si>
+  <si>
+    <t>Expected Response Date</t>
+  </si>
+  <si>
+    <t>Return Date</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>REQ_ PO2_EBL_Electric_Blender_SRS_001.3-1.0</t>
+  </si>
+  <si>
+    <t>Mostafa Ramadan</t>
+  </si>
+  <si>
+    <t>what should be the speed for each state?</t>
+  </si>
+  <si>
+    <t>30/1/2020</t>
+  </si>
+  <si>
+    <t>Speed 1 : from 0% up to 30%. 
 Speed 2: above 30% up to 60%. 
 Speed 3: above  60 % up to 100%.</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Req_ PO2_EBL_Electric_Blender_CYRS_003-1.0</t>
+      <t>Req_ PO2_EBL_Electric_Blender_CYRS_003-1.0</t>
     </r>
     <r>
       <rPr>
@@ -86,26 +85,31 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ahmed Geneidi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is the defined voltage at which the system would be cosidered failed ?</t>
+    <t>Ahmed Geneidi</t>
+  </si>
+  <si>
+    <t>What is the defined voltage at which the system would be cosidered failed ?</t>
   </si>
   <si>
     <t xml:space="preserve">It depends on your motor operating voltage (Min voltage , Max voltage), so under
  Min voltage will consider it as a system failure &amp; above the Max voltage will be
  Considered also as a failure. </t>
+  </si>
+  <si>
+    <t>Req_ PO2_EBL_Electric_Blender_GDD_010-1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the frequency of the PWM is set only once at the beginning of the function so should is be considered a private API? </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -114,22 +118,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="18"/>
       <color rgb="FF333F50"/>
       <name val="Times New Roman"/>
@@ -137,7 +126,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
@@ -145,7 +134,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -153,7 +142,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -164,11 +153,10 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -176,12 +164,25 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -199,7 +200,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -207,89 +208,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -348,35 +312,323 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333F50"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="80.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="70.56"/>
+    <col min="1" max="1" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="115" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+    <col min="6" max="6" width="38" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="70.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="46.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="46.9" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="47.45" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -413,10 +665,10 @@
         <v>10</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="7">
         <v>43854</v>
       </c>
-      <c r="F2" s="7" t="n">
+      <c r="F2" s="7">
         <v>43854</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -426,7 +678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:8" ht="47.45" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -437,28 +689,40 @@
         <v>15</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="7">
         <v>44014</v>
       </c>
-      <c r="F3" s="7" t="n">
+      <c r="F3" s="7">
         <v>44106</v>
       </c>
-      <c r="G3" s="7" t="n">
+      <c r="G3" s="7">
         <v>44076</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="6"/>
+    <row r="4" spans="1:8" ht="47.45" customHeight="1">
+      <c r="A4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="15">
+        <v>44077</v>
+      </c>
+      <c r="F4" s="15">
+        <v>44107</v>
+      </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" ht="47.45" customHeight="1">
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -466,7 +730,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" ht="47.45" customHeight="1">
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -474,7 +738,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:8" ht="47.45" customHeight="1">
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -482,7 +746,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" ht="47.45" customHeight="1">
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -490,7 +754,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" ht="47.45" customHeight="1">
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -498,7 +762,7 @@
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:8" ht="47.45" customHeight="1">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -506,7 +770,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" ht="47.45" customHeight="1">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -514,7 +778,7 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:8" ht="47.45" customHeight="1">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -522,7 +786,7 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" ht="47.45" customHeight="1">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -530,7 +794,7 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" ht="47.45" customHeight="1">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -538,7 +802,7 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" ht="47.45" customHeight="1">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -546,7 +810,7 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" ht="47.45" customHeight="1">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -554,7 +818,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="3:8" ht="47.45" customHeight="1">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -562,7 +826,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="3:8" ht="47.45" customHeight="1">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -570,7 +834,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="3:8" ht="47.45" customHeight="1">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -578,7 +842,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="3:8" ht="47.45" customHeight="1">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -586,7 +850,7 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="3:8" ht="47.45" customHeight="1">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -594,7 +858,7 @@
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="3:8" ht="47.45" customHeight="1">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -602,7 +866,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="3:8" ht="47.45" customHeight="1">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -610,7 +874,7 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="3:8" ht="47.45" customHeight="1">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -618,7 +882,7 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="47.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="3:8" ht="47.45" customHeight="1">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -627,12 +891,7 @@
       <c r="H25" s="6"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>